<commit_message>
minor changes to one of the templates
</commit_message>
<xml_diff>
--- a/templates/miate/MIATE_template.xlsx
+++ b/templates/miate/MIATE_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/tox_Dataharmonier/web/templates/miate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://michiganstate-my.sharepoint.com/personal/naultran_msu_edu/Documents/Documents/Projects/FAIRTox/ToxRSCat/templates/miate/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="381" documentId="13_ncr:1_{312CE87D-C60B-3744-983C-44476127223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1669EAE4-A258-4596-A643-5F781EDB8276}"/>
+  <xr:revisionPtr revIDLastSave="493" documentId="13_ncr:1_{312CE87D-C60B-3744-983C-44476127223B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B848EFBF-03F1-4C69-B2BC-246556C317E4}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{4C05F035-5B59-104F-A647-E8EAB47C9886}"/>
   </bookViews>
   <sheets>
     <sheet name="LinkML_description" sheetId="2" r:id="rId1"/>
@@ -66,7 +66,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="190">
   <si>
     <t>description</t>
   </si>
@@ -185,15 +185,9 @@
     <t>support_id</t>
   </si>
   <si>
-    <t>A textual entity that denotes an study.</t>
-  </si>
-  <si>
     <t>A textual entity that describes an investigation.</t>
   </si>
   <si>
-    <t>the name of the person bearing the data submission contact representative role</t>
-  </si>
-  <si>
     <t>email address of data submission contact</t>
   </si>
   <si>
@@ -212,9 +206,6 @@
     <t>city of data submission contact</t>
   </si>
   <si>
-    <t>state of publication contact</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -254,9 +245,6 @@
     <t>AL, AK, AZ, AR, CA, CO, CT, DE, DC, FL, GA, HI, ID, IL, IN, IA, KS, KY, LA, ME, MD, MA, MI, MN, MS, MO, MT, NB*, *to NE in 1969, NV, NH, NJ, NM, NY, NC, ND, OH, OK, OR, PA, PR, RI, SC, SD, TN, TX, UT, VT, VA, WA, WV, WI, WY</t>
   </si>
   <si>
-    <t>Funding agency</t>
-  </si>
-  <si>
     <t>Funding identifier</t>
   </si>
   <si>
@@ -293,9 +281,6 @@
     <t>P42ES004911</t>
   </si>
   <si>
-    <t>OBI_0001615</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/</t>
   </si>
   <si>
@@ -309,9 +294,6 @@
   </si>
   <si>
     <t>A categorical value specification that specifies the type of study from a list of study types</t>
-  </si>
-  <si>
-    <t>OBI_0500000</t>
   </si>
   <si>
     <t>Study design</t>
@@ -459,12 +441,6 @@
     <t>test_article_administration_duration</t>
   </si>
   <si>
-    <t>euthanasia_time</t>
-  </si>
-  <si>
-    <t>experiment_start_time</t>
-  </si>
-  <si>
     <t>test_article_name</t>
   </si>
   <si>
@@ -528,9 +504,6 @@
     <t>float</t>
   </si>
   <si>
-    <t>##:##</t>
-  </si>
-  <si>
     <t>ad libitum, restricted</t>
   </si>
   <si>
@@ -553,6 +526,117 @@
   </si>
   <si>
     <t>sample_identifier</t>
+  </si>
+  <si>
+    <t>obo:OBI_0001615</t>
+  </si>
+  <si>
+    <t>obo:OBI_0001622</t>
+  </si>
+  <si>
+    <t>A textual entity that denotes an investigation.</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C176230</t>
+  </si>
+  <si>
+    <t>The name of the person acting as a channel for communication between groups or on behalf of a group.</t>
+  </si>
+  <si>
+    <t>obo:IAO_0000708</t>
+  </si>
+  <si>
+    <t>A centrally registered identifier that is issued by ORCID (https://orcid.org/) and used to persistantly identify oneself as a human researcher or contributor.</t>
+  </si>
+  <si>
+    <t>^((?!\.)[\w-_.]*[^.])(@\w+)(\.\w+(\.\w+)?[^.\W])$</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C19711</t>
+  </si>
+  <si>
+    <t>Funding institution</t>
+  </si>
+  <si>
+    <t>A globally unique identifier for a biomedical article, as assigned by PubMed.</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C127797</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C46002</t>
+  </si>
+  <si>
+    <t>^\d{2}:\d{2}$</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C44278</t>
+  </si>
+  <si>
+    <t>^DTXSID\d{7}$</t>
+  </si>
+  <si>
+    <t>state of data submission contact</t>
+  </si>
+  <si>
+    <t>Cage identifier</t>
+  </si>
+  <si>
+    <t>ALPHA-dri, corn cob, wood shavings</t>
+  </si>
+  <si>
+    <t>obo:OBI_0500000</t>
+  </si>
+  <si>
+    <t>http://www.bioassayontology.org/bao#BAO_0020005</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C45293</t>
+  </si>
+  <si>
+    <t>Elapsed time since birth when subjects were assigned to a study.</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C25150</t>
+  </si>
+  <si>
+    <t>experiment_start_zt</t>
+  </si>
+  <si>
+    <t>Experiment start Zeitgeber</t>
+  </si>
+  <si>
+    <t>obo:OBI_0001185</t>
+  </si>
+  <si>
+    <t>obo:PATO_0000047</t>
+  </si>
+  <si>
+    <t>obo:OBI_0000919</t>
+  </si>
+  <si>
+    <t>euthanasia_zt</t>
+  </si>
+  <si>
+    <t>obo:OBI_0000248</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C90377</t>
+  </si>
+  <si>
+    <t>obo:OBI_0000694</t>
+  </si>
+  <si>
+    <t>obo:PATO_0000146</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C88206</t>
+  </si>
+  <si>
+    <t>obo:XCO_0000459</t>
+  </si>
+  <si>
+    <t>obo:NCIT_C90366</t>
   </si>
 </sst>
 </file>
@@ -949,12 +1033,12 @@
       <selection activeCell="A24" sqref="A24:A25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="4" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -971,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -1000,21 +1084,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25A47E7-C24D-194E-BA2A-C4B34C2EC6AD}">
   <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="J84" sqref="J84"/>
+    <sheetView tabSelected="1" zoomScale="79" zoomScaleNormal="79" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="N23" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="R15" sqref="R15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="4" width="21" customWidth="1"/>
-    <col min="5" max="8" width="10.125" customWidth="1"/>
-    <col min="9" max="10" width="15.875" customWidth="1"/>
-    <col min="11" max="13" width="21" customWidth="1"/>
-    <col min="14" max="15" width="14.125" customWidth="1"/>
+    <col min="1" max="2" width="11" customWidth="1"/>
+    <col min="3" max="4" width="21" customWidth="1"/>
+    <col min="5" max="8" width="10.09765625" customWidth="1"/>
+    <col min="9" max="10" width="10" customWidth="1"/>
+    <col min="11" max="12" width="21" customWidth="1"/>
+    <col min="13" max="13" width="12.3984375" customWidth="1"/>
+    <col min="14" max="15" width="14.09765625" customWidth="1"/>
     <col min="16" max="18" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -1070,70 +1159,79 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>30</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C2" t="s">
         <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L2" t="s">
-        <v>39</v>
+        <v>155</v>
+      </c>
+      <c r="O2" t="b">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>71</v>
       </c>
       <c r="R2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
       </c>
       <c r="D3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="L3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P3" t="s">
-        <v>75</v>
+        <v>153</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="E4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I4" t="b">
         <v>1</v>
@@ -1142,33 +1240,39 @@
         <v>1</v>
       </c>
       <c r="L4" t="s">
-        <v>41</v>
+        <v>157</v>
       </c>
       <c r="N4" t="b">
         <v>1</v>
       </c>
+      <c r="P4" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="R4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C5" t="s">
         <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="I5" t="b">
         <v>1</v>
@@ -1176,28 +1280,40 @@
       <c r="J5" t="b">
         <v>1</v>
       </c>
+      <c r="L5" t="s">
+        <v>159</v>
+      </c>
       <c r="O5" t="b">
         <v>1</v>
       </c>
+      <c r="P5" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="R5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
       <c r="B6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>29</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>147</v>
+        <v>139</v>
+      </c>
+      <c r="H6" t="s">
+        <v>160</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -1206,30 +1322,30 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="N6" t="b">
         <v>1</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="E7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I7" t="b">
         <v>1</v>
@@ -1238,27 +1354,27 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="R7">
         <v>5178842054</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="E8" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I8" t="b">
         <v>1</v>
@@ -1267,27 +1383,27 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="R8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E9" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I9" t="b">
         <v>1</v>
@@ -1296,27 +1412,27 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="R9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="E10" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I10" t="b">
         <v>1</v>
@@ -1325,27 +1441,27 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="R10">
         <v>48824</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s">
         <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E11" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I11" t="b">
         <v>1</v>
@@ -1354,27 +1470,27 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="R11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>36</v>
       </c>
       <c r="D12" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="E12" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I12" t="b">
         <v>1</v>
@@ -1383,30 +1499,30 @@
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L12" t="s">
-        <v>48</v>
+        <v>169</v>
       </c>
       <c r="R12" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>30</v>
       </c>
       <c r="B13" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" t="s">
         <v>37</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
+        <v>162</v>
       </c>
       <c r="E13" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I13" t="b">
         <v>1</v>
@@ -1417,25 +1533,31 @@
       <c r="N13" t="b">
         <v>1</v>
       </c>
+      <c r="P13" t="s">
+        <v>161</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="R13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C14" t="s">
         <v>38</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E14" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I14" t="b">
         <v>1</v>
@@ -1447,24 +1569,24 @@
         <v>1</v>
       </c>
       <c r="R14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>30</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D15" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I15" t="b">
         <v>1</v>
@@ -1473,21 +1595,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>30</v>
       </c>
       <c r="B16" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E16" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I16" t="b">
         <v>1</v>
@@ -1496,392 +1618,467 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I17" t="b">
+        <v>1</v>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
+      </c>
+      <c r="L17" t="s">
+        <v>163</v>
+      </c>
+      <c r="P17" t="s">
+        <v>164</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E18" t="s">
+        <v>139</v>
+      </c>
+      <c r="O18" t="b">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>90</v>
+      </c>
+      <c r="B19" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" t="s">
         <v>95</v>
       </c>
-      <c r="D17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" t="s">
-        <v>147</v>
-      </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>96</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="E19" t="s">
+        <v>139</v>
+      </c>
+      <c r="O19" t="b">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" t="s">
+        <v>72</v>
+      </c>
+      <c r="D20" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" t="s">
+        <v>146</v>
+      </c>
+      <c r="K20" t="s">
+        <v>78</v>
+      </c>
+      <c r="L20" t="s">
+        <v>74</v>
+      </c>
+      <c r="P20" t="s">
+        <v>172</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>90</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" t="s">
+        <v>73</v>
+      </c>
+      <c r="D21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E21" t="s">
+        <v>146</v>
+      </c>
+      <c r="K21" t="s">
+        <v>79</v>
+      </c>
+      <c r="L21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" t="s">
+        <v>92</v>
+      </c>
+      <c r="C22" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="s">
+        <v>146</v>
+      </c>
+      <c r="K22" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>90</v>
+      </c>
+      <c r="B23" t="s">
+        <v>92</v>
+      </c>
+      <c r="C23" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" t="s">
+        <v>146</v>
+      </c>
+      <c r="K23" t="s">
+        <v>84</v>
+      </c>
+      <c r="O23" t="b">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>174</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>139</v>
+      </c>
+      <c r="O24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B25" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" t="s">
+        <v>103</v>
+      </c>
+      <c r="E25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C26" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" t="s">
+        <v>140</v>
+      </c>
+      <c r="L26" t="s">
+        <v>175</v>
+      </c>
+      <c r="P26" t="s">
+        <v>176</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27" t="s">
+        <v>105</v>
+      </c>
+      <c r="C27" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>90</v>
+      </c>
+      <c r="B28" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D28" t="s">
+        <v>178</v>
+      </c>
+      <c r="E28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" t="s">
+        <v>105</v>
+      </c>
+      <c r="C29" t="s">
+        <v>110</v>
+      </c>
+      <c r="E29" t="s">
+        <v>139</v>
+      </c>
+      <c r="K29" t="s">
+        <v>141</v>
+      </c>
+      <c r="O29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" t="s">
+        <v>180</v>
+      </c>
+      <c r="Q29" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>90</v>
+      </c>
+      <c r="B30" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" t="s">
+        <v>111</v>
+      </c>
+      <c r="E30" t="s">
+        <v>139</v>
+      </c>
+      <c r="K30" t="s">
+        <v>142</v>
+      </c>
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q30" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>105</v>
+      </c>
+      <c r="C31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>90</v>
+      </c>
+      <c r="B32" t="s">
+        <v>105</v>
+      </c>
+      <c r="C32" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>90</v>
+      </c>
+      <c r="B33" t="s">
+        <v>105</v>
+      </c>
+      <c r="C33" t="s">
+        <v>182</v>
+      </c>
+      <c r="E33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" t="s">
+        <v>109</v>
+      </c>
+      <c r="E34" t="s">
+        <v>139</v>
+      </c>
+      <c r="K34" t="s">
+        <v>143</v>
+      </c>
+      <c r="P34" t="s">
+        <v>181</v>
+      </c>
+      <c r="Q34" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" t="s">
+        <v>97</v>
+      </c>
+      <c r="C35" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>90</v>
+      </c>
+      <c r="B36" t="s">
+        <v>97</v>
+      </c>
+      <c r="C36" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" t="s">
         <v>100</v>
       </c>
-      <c r="C18" t="s">
-        <v>99</v>
-      </c>
-      <c r="E18" t="s">
-        <v>147</v>
-      </c>
-      <c r="O18" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>96</v>
-      </c>
-      <c r="B19" t="s">
-        <v>100</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E37" t="s">
+        <v>146</v>
+      </c>
+      <c r="K37" t="s">
+        <v>171</v>
+      </c>
+      <c r="P37" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q37" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s">
         <v>101</v>
       </c>
-      <c r="E19" t="s">
-        <v>147</v>
-      </c>
-      <c r="O19" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>96</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" t="s">
-        <v>82</v>
-      </c>
-      <c r="E20" t="s">
-        <v>147</v>
-      </c>
-      <c r="K20" t="s">
-        <v>84</v>
-      </c>
-      <c r="L20" t="s">
-        <v>79</v>
-      </c>
-      <c r="P20" t="s">
-        <v>81</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>96</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" t="s">
-        <v>78</v>
-      </c>
-      <c r="D21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E21" t="s">
-        <v>147</v>
-      </c>
-      <c r="K21" t="s">
-        <v>85</v>
-      </c>
-      <c r="L21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>88</v>
-      </c>
-      <c r="E22" t="s">
-        <v>147</v>
-      </c>
-      <c r="K22" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>96</v>
-      </c>
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E23" t="s">
-        <v>147</v>
-      </c>
-      <c r="K23" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>96</v>
-      </c>
-      <c r="B24" t="s">
-        <v>111</v>
-      </c>
-      <c r="C24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E24" t="s">
-        <v>147</v>
-      </c>
-      <c r="O24" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" t="s">
-        <v>111</v>
-      </c>
-      <c r="C25" t="s">
-        <v>109</v>
-      </c>
-      <c r="E25" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>96</v>
-      </c>
-      <c r="B26" t="s">
-        <v>111</v>
-      </c>
-      <c r="C26" t="s">
-        <v>112</v>
-      </c>
-      <c r="E26" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>96</v>
-      </c>
-      <c r="B27" t="s">
-        <v>111</v>
-      </c>
-      <c r="C27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E27" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>96</v>
-      </c>
-      <c r="B28" t="s">
-        <v>111</v>
-      </c>
-      <c r="C28" t="s">
-        <v>131</v>
-      </c>
-      <c r="E28" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>96</v>
-      </c>
-      <c r="B29" t="s">
-        <v>111</v>
-      </c>
-      <c r="C29" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" t="s">
-        <v>147</v>
-      </c>
-      <c r="K29" t="s">
-        <v>149</v>
-      </c>
-      <c r="O29" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>96</v>
-      </c>
-      <c r="B30" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" t="s">
-        <v>147</v>
-      </c>
-      <c r="K30" t="s">
-        <v>150</v>
-      </c>
-      <c r="O30" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C31" t="s">
-        <v>118</v>
-      </c>
-      <c r="E31" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>96</v>
-      </c>
-      <c r="B32" t="s">
-        <v>111</v>
-      </c>
-      <c r="C32" t="s">
-        <v>114</v>
-      </c>
-      <c r="E32" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>96</v>
-      </c>
-      <c r="B33" t="s">
-        <v>111</v>
-      </c>
-      <c r="C33" t="s">
-        <v>130</v>
-      </c>
-      <c r="E33" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>96</v>
-      </c>
-      <c r="B34" t="s">
-        <v>111</v>
-      </c>
-      <c r="C34" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" t="s">
-        <v>147</v>
-      </c>
-      <c r="K34" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>96</v>
-      </c>
-      <c r="B35" t="s">
-        <v>103</v>
-      </c>
-      <c r="C35" t="s">
-        <v>110</v>
-      </c>
-      <c r="E35" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>96</v>
-      </c>
-      <c r="B36" t="s">
-        <v>103</v>
-      </c>
-      <c r="C36" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" t="s">
-        <v>103</v>
-      </c>
-      <c r="C37" t="s">
-        <v>106</v>
-      </c>
-      <c r="E37" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>96</v>
-      </c>
-      <c r="B38" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" t="s">
-        <v>107</v>
-      </c>
       <c r="E38" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B39" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C39" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -1889,19 +2086,25 @@
       <c r="G39">
         <v>50</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P39" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q39" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C40" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E40" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="F40">
         <v>0</v>
@@ -1909,213 +2112,255 @@
       <c r="G40">
         <v>100</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P40" t="s">
+        <v>187</v>
+      </c>
+      <c r="Q40" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B41" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="E41" t="s">
+        <v>139</v>
+      </c>
+      <c r="H41" t="s">
+        <v>166</v>
+      </c>
+      <c r="P41" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q41" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>90</v>
+      </c>
+      <c r="B42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C42" t="s">
+        <v>104</v>
+      </c>
+      <c r="E42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" t="s">
+        <v>98</v>
+      </c>
+      <c r="C43" t="s">
+        <v>113</v>
+      </c>
+      <c r="E43" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C44" t="s">
+        <v>114</v>
+      </c>
+      <c r="E44" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" t="s">
+        <v>98</v>
+      </c>
+      <c r="C45" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" t="s">
+        <v>139</v>
+      </c>
+      <c r="P45" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" t="s">
+        <v>131</v>
+      </c>
+      <c r="E47" t="s">
+        <v>139</v>
+      </c>
+      <c r="P47" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q47" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>90</v>
+      </c>
+      <c r="B48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" t="s">
+        <v>132</v>
+      </c>
+      <c r="E48" t="s">
+        <v>146</v>
+      </c>
+      <c r="K48" t="s">
+        <v>145</v>
+      </c>
+      <c r="P48" t="s">
+        <v>185</v>
+      </c>
+      <c r="Q48" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="B49" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" t="s">
+        <v>104</v>
+      </c>
+      <c r="E49" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>90</v>
+      </c>
+      <c r="B50" t="s">
+        <v>117</v>
+      </c>
+      <c r="C50" t="s">
+        <v>118</v>
+      </c>
+      <c r="E50" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>90</v>
+      </c>
+      <c r="B51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" t="s">
+        <v>119</v>
+      </c>
+      <c r="E51" t="s">
+        <v>144</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+      <c r="J51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>90</v>
+      </c>
+      <c r="B52" t="s">
+        <v>117</v>
+      </c>
+      <c r="C52" t="s">
+        <v>120</v>
+      </c>
+      <c r="E52" t="s">
+        <v>146</v>
+      </c>
+      <c r="K52" t="s">
         <v>147</v>
       </c>
-      <c r="H41" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>96</v>
-      </c>
-      <c r="B42" t="s">
-        <v>104</v>
-      </c>
-      <c r="C42" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>96</v>
-      </c>
-      <c r="B43" t="s">
-        <v>104</v>
-      </c>
-      <c r="C43" t="s">
-        <v>119</v>
-      </c>
-      <c r="E43" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>96</v>
-      </c>
-      <c r="B44" t="s">
-        <v>104</v>
-      </c>
-      <c r="C44" t="s">
-        <v>120</v>
-      </c>
-      <c r="E44" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>96</v>
-      </c>
-      <c r="B45" t="s">
-        <v>104</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="P52" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q52" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" t="s">
         <v>121</v>
       </c>
-      <c r="E45" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="E53" t="s">
+        <v>146</v>
+      </c>
+      <c r="K53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>90</v>
+      </c>
+      <c r="B54" t="s">
+        <v>117</v>
+      </c>
+      <c r="C54" t="s">
         <v>122</v>
       </c>
-      <c r="E46" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>96</v>
-      </c>
-      <c r="B47" t="s">
-        <v>104</v>
-      </c>
-      <c r="C47" t="s">
-        <v>139</v>
-      </c>
-      <c r="E47" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="E54" t="s">
         <v>140</v>
-      </c>
-      <c r="E48" t="s">
-        <v>155</v>
-      </c>
-      <c r="K48" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>96</v>
-      </c>
-      <c r="B49" t="s">
-        <v>123</v>
-      </c>
-      <c r="C49" t="s">
-        <v>110</v>
-      </c>
-      <c r="E49" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" t="s">
-        <v>123</v>
-      </c>
-      <c r="C50" t="s">
-        <v>124</v>
-      </c>
-      <c r="E50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>96</v>
-      </c>
-      <c r="B51" t="s">
-        <v>123</v>
-      </c>
-      <c r="C51" t="s">
-        <v>125</v>
-      </c>
-      <c r="E51" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>96</v>
-      </c>
-      <c r="B52" t="s">
-        <v>123</v>
-      </c>
-      <c r="C52" t="s">
-        <v>126</v>
-      </c>
-      <c r="E52" t="s">
-        <v>155</v>
-      </c>
-      <c r="K52" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>96</v>
-      </c>
-      <c r="B53" t="s">
-        <v>123</v>
-      </c>
-      <c r="C53" t="s">
-        <v>127</v>
-      </c>
-      <c r="E53" t="s">
-        <v>155</v>
-      </c>
-      <c r="K53" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>96</v>
-      </c>
-      <c r="B54" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" t="s">
-        <v>128</v>
-      </c>
-      <c r="E54" t="s">
-        <v>148</v>
       </c>
       <c r="F54">
         <v>0</v>
@@ -2124,184 +2369,214 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="B55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C55" t="s">
         <v>123</v>
       </c>
-      <c r="C55" t="s">
-        <v>129</v>
-      </c>
       <c r="E55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" t="s">
+        <v>117</v>
+      </c>
+      <c r="C56" t="s">
+        <v>124</v>
+      </c>
+      <c r="E56" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57" t="s">
+        <v>117</v>
+      </c>
+      <c r="C57" t="s">
+        <v>125</v>
+      </c>
+      <c r="E57" t="s">
+        <v>139</v>
+      </c>
+      <c r="H57" t="s">
+        <v>168</v>
+      </c>
+      <c r="I57" t="b">
+        <v>1</v>
+      </c>
+      <c r="J57" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" t="s">
+        <v>139</v>
+      </c>
+      <c r="I58" t="b">
+        <v>1</v>
+      </c>
+      <c r="J58" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>90</v>
+      </c>
+      <c r="B59" t="s">
+        <v>117</v>
+      </c>
+      <c r="C59" t="s">
+        <v>127</v>
+      </c>
+      <c r="E59" t="s">
+        <v>139</v>
+      </c>
+      <c r="H59" t="s">
+        <v>168</v>
+      </c>
+      <c r="I59" t="b">
+        <v>1</v>
+      </c>
+      <c r="J59" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>91</v>
+      </c>
+      <c r="B60" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" t="s">
+        <v>95</v>
+      </c>
+      <c r="E60" t="s">
+        <v>139</v>
+      </c>
+      <c r="I60" t="b">
+        <v>1</v>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>91</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" t="s">
+        <v>102</v>
+      </c>
+      <c r="E61" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>91</v>
+      </c>
+      <c r="B62" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>96</v>
-      </c>
-      <c r="B56" t="s">
-        <v>123</v>
-      </c>
-      <c r="C56" t="s">
-        <v>132</v>
-      </c>
-      <c r="E56" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>96</v>
-      </c>
-      <c r="B57" t="s">
-        <v>123</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="E62" t="s">
+        <v>139</v>
+      </c>
+      <c r="M62" t="b">
+        <v>1</v>
+      </c>
+      <c r="O62" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>91</v>
+      </c>
+      <c r="B63" t="s">
+        <v>138</v>
+      </c>
+      <c r="C63" t="s">
+        <v>104</v>
+      </c>
+      <c r="E63" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64" t="s">
+        <v>138</v>
+      </c>
+      <c r="C64" t="s">
         <v>133</v>
       </c>
-      <c r="E57" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>96</v>
-      </c>
-      <c r="B58" t="s">
-        <v>123</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="E64" t="s">
+        <v>139</v>
+      </c>
+      <c r="K64" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>91</v>
+      </c>
+      <c r="B65" t="s">
+        <v>138</v>
+      </c>
+      <c r="C65" t="s">
         <v>134</v>
       </c>
-      <c r="E58" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>96</v>
-      </c>
-      <c r="B59" t="s">
-        <v>123</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="E65" t="s">
+        <v>139</v>
+      </c>
+      <c r="K65" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" t="s">
+        <v>138</v>
+      </c>
+      <c r="C66" t="s">
         <v>135</v>
       </c>
-      <c r="E59" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>97</v>
-      </c>
-      <c r="B60" t="s">
-        <v>100</v>
-      </c>
-      <c r="C60" t="s">
-        <v>101</v>
-      </c>
-      <c r="E60" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>97</v>
-      </c>
-      <c r="B61" t="s">
-        <v>100</v>
-      </c>
-      <c r="C61" t="s">
-        <v>108</v>
-      </c>
-      <c r="E61" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>97</v>
-      </c>
-      <c r="B62" t="s">
-        <v>100</v>
-      </c>
-      <c r="C62" t="s">
-        <v>161</v>
-      </c>
-      <c r="E62" t="s">
-        <v>147</v>
-      </c>
-      <c r="M62" t="b">
-        <v>1</v>
-      </c>
-      <c r="O62" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>97</v>
-      </c>
-      <c r="B63" t="s">
-        <v>146</v>
-      </c>
-      <c r="C63" t="s">
-        <v>110</v>
-      </c>
-      <c r="E63" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>97</v>
-      </c>
-      <c r="B64" t="s">
-        <v>146</v>
-      </c>
-      <c r="C64" t="s">
-        <v>141</v>
-      </c>
-      <c r="E64" t="s">
-        <v>147</v>
-      </c>
-      <c r="K64" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>97</v>
-      </c>
-      <c r="B65" t="s">
-        <v>146</v>
-      </c>
-      <c r="C65" t="s">
-        <v>142</v>
-      </c>
-      <c r="E65" t="s">
-        <v>147</v>
-      </c>
-      <c r="K65" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>97</v>
-      </c>
-      <c r="B66" t="s">
-        <v>146</v>
-      </c>
-      <c r="C66" t="s">
-        <v>143</v>
-      </c>
       <c r="E66" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I66" t="b">
         <v>1</v>
@@ -2310,35 +2585,35 @@
         <v>1</v>
       </c>
       <c r="K66" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C67" t="s">
+        <v>136</v>
+      </c>
+      <c r="E67" t="s">
         <v>144</v>
       </c>
-      <c r="E67" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C68" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="E68" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>
@@ -2346,8 +2621,30 @@
     <hyperlink ref="R6" r:id="rId1" xr:uid="{6730DB56-29A4-4368-838D-F7C90E1BA941}"/>
     <hyperlink ref="Q3" r:id="rId2" xr:uid="{D67885DB-07C1-48D6-9182-296C8764ACAA}"/>
     <hyperlink ref="Q20" r:id="rId3" xr:uid="{62B2D977-4DB4-4ACB-B1F4-86B39E729F12}"/>
+    <hyperlink ref="Q2" r:id="rId4" xr:uid="{3E4ADA5D-25DC-4FCF-9AD6-84FFBF29DD54}"/>
+    <hyperlink ref="Q4" r:id="rId5" xr:uid="{77C6100B-CB8B-45BC-B9F4-81B72C4CDBBE}"/>
+    <hyperlink ref="Q5" r:id="rId6" xr:uid="{983294F6-1794-48BA-A4EE-69E1E5B73B29}"/>
+    <hyperlink ref="Q13" r:id="rId7" xr:uid="{5F4DB769-A8DA-4A96-B09C-E6FF792A6727}"/>
+    <hyperlink ref="Q17" r:id="rId8" xr:uid="{CE8CEF44-F1F7-4EC2-8E60-7E851335A50D}"/>
+    <hyperlink ref="Q18" r:id="rId9" xr:uid="{5537B217-12A2-4369-87D2-C5E2A4AC65D4}"/>
+    <hyperlink ref="Q19" r:id="rId10" xr:uid="{601611FE-DEAE-44CA-B260-AD4FF56D97E4}"/>
+    <hyperlink ref="Q52" r:id="rId11" xr:uid="{ECB42EBD-C556-4586-BBCA-16A58E127BF1}"/>
+    <hyperlink ref="Q22" r:id="rId12" location="BAO_0020005" xr:uid="{37B5E50D-20D7-44B7-BF1B-86D0E401725C}"/>
+    <hyperlink ref="Q23" r:id="rId13" xr:uid="{DF0D288C-738F-4EAF-8911-7FEBFED5730E}"/>
+    <hyperlink ref="Q26" r:id="rId14" xr:uid="{E4FCB884-4466-4FA3-98B9-00D3E4577E54}"/>
+    <hyperlink ref="Q30" r:id="rId15" xr:uid="{96FFD262-981A-4D2A-8B92-2223FADC171E}"/>
+    <hyperlink ref="Q29" r:id="rId16" xr:uid="{498AD441-F42E-48F4-9FE0-8E0EDAC27CB2}"/>
+    <hyperlink ref="Q34" r:id="rId17" xr:uid="{3F93E517-A771-4277-B1C4-0D484378F3C6}"/>
+    <hyperlink ref="Q45" r:id="rId18" xr:uid="{5A4F09E9-4852-4FEA-8962-95A99CB5321D}"/>
+    <hyperlink ref="Q48" r:id="rId19" xr:uid="{4C5D9327-68A9-4796-890F-96EEDD7AB960}"/>
+    <hyperlink ref="Q47" r:id="rId20" xr:uid="{D1DF37D3-4D5A-462E-8C75-798FDCCDA9E3}"/>
+    <hyperlink ref="Q39" r:id="rId21" xr:uid="{8752855E-5008-493E-8E83-E2F603B0407D}"/>
+    <hyperlink ref="Q40" r:id="rId22" xr:uid="{6613030B-8CAB-4FB8-AF4D-7A3FC2B4FE5F}"/>
+    <hyperlink ref="Q41" r:id="rId23" xr:uid="{B9400ADF-E07A-407E-8FA2-0F94CB143507}"/>
+    <hyperlink ref="Q37" r:id="rId24" xr:uid="{19AAC4D7-5401-4799-9C07-9F3476E72451}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
+  <legacyDrawing r:id="rId26"/>
 </worksheet>
 </file>
</xml_diff>